<commit_message>
# ultima versión de datos
</commit_message>
<xml_diff>
--- a/www/bd/bd_indice_impunidad.xlsx
+++ b/www/bd/bd_indice_impunidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriacampuzano/Documents/MEXICO EVALUA/DashboardsHallazgos/dashboardhallazgos/www/bd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17906018-0AB6-0E49-876E-0630E0CD8DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1284CD0-902F-5144-AD2D-F3953EF6A66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{5CA585DF-E9E5-F747-9958-22FD88E06556}"/>
   </bookViews>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D00630-DBEC-794C-81D5-E3B430488D04}">
   <dimension ref="A1:E793"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="240" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A846" workbookViewId="0">
+      <selection activeCell="C326" sqref="C326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="E162" s="6">
         <f ca="1">RAND()*100</f>
-        <v>44.350343285648151</v>
+        <v>5.6021727602346587</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -3364,7 +3364,7 @@
       </c>
       <c r="E163" s="6">
         <f t="shared" ref="E163:E191" ca="1" si="0">RAND()*100</f>
-        <v>30.734937263448238</v>
+        <v>70.563823323705932</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -3382,7 +3382,7 @@
       </c>
       <c r="E164" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8287794788154965</v>
+        <v>43.179495708080765</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="E165" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>41.637862359465203</v>
+        <v>31.456824691813889</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="E166" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>26.965431292047548</v>
+        <v>9.3880331489299973</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="E167" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>12.504545629927499</v>
+        <v>45.166937809541544</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -3454,7 +3454,7 @@
       </c>
       <c r="E168" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>82.003343277012206</v>
+        <v>21.809625285570043</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -3472,7 +3472,7 @@
       </c>
       <c r="E169" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>22.245790510963047</v>
+        <v>26.529616546214683</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -3490,7 +3490,7 @@
       </c>
       <c r="E170" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>78.321811086160423</v>
+        <v>14.20915368163601</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="E171" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>50.852216416344675</v>
+        <v>28.820410089698491</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -3526,7 +3526,7 @@
       </c>
       <c r="E172" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>72.485802697478164</v>
+        <v>85.412499091058663</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -3544,7 +3544,7 @@
       </c>
       <c r="E173" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>99.715631966044171</v>
+        <v>13.024260334974514</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="E174" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>52.927353549754649</v>
+        <v>53.851799552628712</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -3580,7 +3580,7 @@
       </c>
       <c r="E175" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>36.051893139918135</v>
+        <v>93.480321008248865</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -3598,7 +3598,7 @@
       </c>
       <c r="E176" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>94.043445259848781</v>
+        <v>43.916548436180733</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -3616,7 +3616,7 @@
       </c>
       <c r="E177" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>46.688202890165456</v>
+        <v>87.410638285820625</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -3634,7 +3634,7 @@
       </c>
       <c r="E178" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>11.014045671013806</v>
+        <v>94.988531082419016</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -3652,7 +3652,7 @@
       </c>
       <c r="E179" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>14.34271960047646</v>
+        <v>74.090076340537834</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
@@ -3670,7 +3670,7 @@
       </c>
       <c r="E180" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>64.807816586641152</v>
+        <v>22.963400892665941</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="E181" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>38.31245160661706</v>
+        <v>72.517979622696231</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -3706,7 +3706,7 @@
       </c>
       <c r="E182" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9771815060298081</v>
+        <v>32.57164266106448</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
@@ -3724,7 +3724,7 @@
       </c>
       <c r="E183" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>81.060888706192287</v>
+        <v>68.424757907689511</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -3742,7 +3742,7 @@
       </c>
       <c r="E184" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>64.758199287825406</v>
+        <v>96.063929159522814</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -3760,7 +3760,7 @@
       </c>
       <c r="E185" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>36.779811626222724</v>
+        <v>64.69136418982356</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
@@ -3778,7 +3778,7 @@
       </c>
       <c r="E186" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>30.9685262800811</v>
+        <v>32.118919204412499</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
@@ -3796,7 +3796,7 @@
       </c>
       <c r="E187" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>53.3412377619618</v>
+        <v>42.646821326186199</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
@@ -3814,7 +3814,7 @@
       </c>
       <c r="E188" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5855206228201264</v>
+        <v>57.794554208065627</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
@@ -3832,7 +3832,7 @@
       </c>
       <c r="E189" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8894250821957019</v>
+        <v>38.843784704095377</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
@@ -3850,7 +3850,7 @@
       </c>
       <c r="E190" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>74.632378287301677</v>
+        <v>47.925131069194592</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -3868,7 +3868,7 @@
       </c>
       <c r="E191" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>35.569402691087035</v>
+        <v>98.709754253916699</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -6026,6 +6026,9 @@
       <c r="D318" s="1">
         <v>2022</v>
       </c>
+      <c r="E318" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
@@ -6040,6 +6043,9 @@
       <c r="D319" s="1">
         <v>2022</v>
       </c>
+      <c r="E319" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
@@ -8742,7 +8748,7 @@
       </c>
       <c r="E478" s="3">
         <f ca="1">RAND()*100</f>
-        <v>7.5991807802277656</v>
+        <v>77.404573339186783</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.2">
@@ -8760,7 +8766,7 @@
       </c>
       <c r="E479" s="3">
         <f t="shared" ref="E479:E507" ca="1" si="1">RAND()*100</f>
-        <v>44.958119105139495</v>
+        <v>10.162445657334073</v>
       </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.2">
@@ -8778,7 +8784,7 @@
       </c>
       <c r="E480" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>22.82669959772079</v>
+        <v>13.138504268815366</v>
       </c>
     </row>
     <row r="481" spans="1:5" x14ac:dyDescent="0.2">
@@ -8796,7 +8802,7 @@
       </c>
       <c r="E481" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.741049516784964</v>
+        <v>60.119363169354102</v>
       </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.2">
@@ -8814,7 +8820,7 @@
       </c>
       <c r="E482" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7569313084981775</v>
+        <v>65.852369008741391</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.2">
@@ -8832,7 +8838,7 @@
       </c>
       <c r="E483" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>62.317453114296839</v>
+        <v>94.208225862712652</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.2">
@@ -8850,7 +8856,7 @@
       </c>
       <c r="E484" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>83.388291643206287</v>
+        <v>31.709898484829914</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.2">
@@ -8868,7 +8874,7 @@
       </c>
       <c r="E485" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>60.582989777341275</v>
+        <v>11.623531519064123</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.2">
@@ -8886,7 +8892,7 @@
       </c>
       <c r="E486" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>17.212783412654929</v>
+        <v>26.979225494042236</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.2">
@@ -8904,7 +8910,7 @@
       </c>
       <c r="E487" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0047169857982752</v>
+        <v>96.606466962127698</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.2">
@@ -8922,7 +8928,7 @@
       </c>
       <c r="E488" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>80.727220082734561</v>
+        <v>9.4114139566299659</v>
       </c>
     </row>
     <row r="489" spans="1:5" x14ac:dyDescent="0.2">
@@ -8940,7 +8946,7 @@
       </c>
       <c r="E489" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5590072858516231</v>
+        <v>53.62269763960812</v>
       </c>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.2">
@@ -8958,7 +8964,7 @@
       </c>
       <c r="E490" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12789167489603015</v>
+        <v>1.3740947351270072</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.2">
@@ -8976,7 +8982,7 @@
       </c>
       <c r="E491" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>55.693022341724927</v>
+        <v>20.414041276833061</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.2">
@@ -8994,7 +9000,7 @@
       </c>
       <c r="E492" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>49.221061400965397</v>
+        <v>69.127092781811612</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.2">
@@ -9012,7 +9018,7 @@
       </c>
       <c r="E493" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>40.665605688721186</v>
+        <v>65.080411150038657</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.2">
@@ -9030,7 +9036,7 @@
       </c>
       <c r="E494" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>47.456343643318391</v>
+        <v>74.538909742623076</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.2">
@@ -9048,7 +9054,7 @@
       </c>
       <c r="E495" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>88.03442916364655</v>
+        <v>52.268034873632296</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.2">
@@ -9066,7 +9072,7 @@
       </c>
       <c r="E496" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>87.997806336188319</v>
+        <v>38.834417045042578</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.2">
@@ -9084,7 +9090,7 @@
       </c>
       <c r="E497" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>71.920526832848168</v>
+        <v>45.319683363237615</v>
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.2">
@@ -9102,7 +9108,7 @@
       </c>
       <c r="E498" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>31.425215407662609</v>
+        <v>79.620706179467859</v>
       </c>
     </row>
     <row r="499" spans="1:5" x14ac:dyDescent="0.2">
@@ -9120,7 +9126,7 @@
       </c>
       <c r="E499" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>34.22388752295511</v>
+        <v>35.290141903983333</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.2">
@@ -9138,7 +9144,7 @@
       </c>
       <c r="E500" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>86.218093161561455</v>
+        <v>76.530012952034411</v>
       </c>
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.2">
@@ -9156,7 +9162,7 @@
       </c>
       <c r="E501" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>19.490944618767926</v>
+        <v>3.0651207676107628</v>
       </c>
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.2">
@@ -9174,7 +9180,7 @@
       </c>
       <c r="E502" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>93.564589615374899</v>
+        <v>36.57541302645938</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.2">
@@ -9192,7 +9198,7 @@
       </c>
       <c r="E503" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>36.346786794374573</v>
+        <v>59.850628088976919</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.2">
@@ -9210,7 +9216,7 @@
       </c>
       <c r="E504" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1170912124833503</v>
+        <v>60.880759911922368</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.2">
@@ -9228,7 +9234,7 @@
       </c>
       <c r="E505" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>70.314810738923555</v>
+        <v>40.277538683938772</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.2">
@@ -9246,7 +9252,7 @@
       </c>
       <c r="E506" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>78.983255132882462</v>
+        <v>54.242299487986855</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.2">
@@ -9264,7 +9270,7 @@
       </c>
       <c r="E507" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>69.190541517878472</v>
+        <v>14.700783521092564</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>